<commit_message>
Sorted out some basic math for new stats
</commit_message>
<xml_diff>
--- a/Classes.xlsx
+++ b/Classes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GameThing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07ABD69-822B-47BE-BCCB-2F79B25A384B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF6CDBB-19C6-41EF-BCC6-82ECA490705B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B43DC27E-312F-4ABF-897F-B8623FBBEEFC}"/>
   </bookViews>
@@ -974,9 +974,6 @@
     <t>Gust</t>
   </si>
   <si>
-    <t>Play one less card next, give all characters within 3 +1 Defense for 3 turns.</t>
-  </si>
-  <si>
     <t>Ready</t>
   </si>
   <si>
@@ -1308,6 +1305,9 @@
   </si>
   <si>
     <t>Int, Damage, Magic</t>
+  </si>
+  <si>
+    <t>Play one less card next, give all characters within 3 +100% Defense for 3 turns.</t>
   </si>
 </sst>
 </file>
@@ -1688,19 +1688,19 @@
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>95</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>36</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>100</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>101</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>102</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>103</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>85</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>104</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -2197,62 +2197,62 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>39</v>
       </c>
@@ -2267,21 +2267,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86656FBC-7A08-4294-A713-C6003B80014C}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>135</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
         <v>274</v>
@@ -2313,13 +2313,13 @@
         <v>271</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
         <v>274</v>
@@ -2337,7 +2337,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
         <v>274</v>
@@ -2355,7 +2355,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
         <v>274</v>
@@ -2373,7 +2373,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="6" t="s">
         <v>274</v>
@@ -2385,13 +2385,13 @@
         <v>272</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="6" t="s">
         <v>274</v>
@@ -2403,13 +2403,13 @@
         <v>273</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="6" t="s">
         <v>18</v>
@@ -2427,7 +2427,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
@@ -2445,7 +2445,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
@@ -2463,7 +2463,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -2481,7 +2481,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6" t="s">
         <v>20</v>
@@ -2499,7 +2499,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="6" t="s">
         <v>20</v>
@@ -2517,13 +2517,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="C14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -2534,46 +2534,46 @@
         <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>330</v>
+      </c>
+      <c r="D17" t="s">
+        <v>386</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>331</v>
       </c>
-      <c r="D17" t="s">
-        <v>387</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>332</v>
       </c>
-      <c r="D18" t="s">
-        <v>333</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -2584,46 +2584,46 @@
         <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>240</v>
       </c>
       <c r="D20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>333</v>
+      </c>
+      <c r="D21" t="s">
+        <v>354</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>338</v>
+      </c>
+      <c r="D22" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>334</v>
-      </c>
-      <c r="D21" t="s">
-        <v>355</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>339</v>
-      </c>
-      <c r="D22" t="s">
-        <v>354</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -2634,46 +2634,46 @@
         <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>249</v>
       </c>
       <c r="D24" t="s">
+        <v>377</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D25" t="s">
         <v>335</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>336</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>337</v>
       </c>
-      <c r="D26" t="s">
-        <v>338</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -2684,46 +2684,46 @@
         <v>155</v>
       </c>
       <c r="D27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D28" t="s">
         <v>288</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" t="s">
+        <v>339</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>342</v>
+      </c>
+      <c r="D30" t="s">
+        <v>343</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>327</v>
-      </c>
-      <c r="D29" t="s">
-        <v>340</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>343</v>
-      </c>
-      <c r="D30" t="s">
-        <v>344</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>140</v>
       </c>
@@ -2734,46 +2734,46 @@
         <v>280</v>
       </c>
       <c r="D31" t="s">
+        <v>383</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>344</v>
+      </c>
+      <c r="D33" t="s">
+        <v>364</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>345</v>
       </c>
-      <c r="D33" t="s">
-        <v>365</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>346</v>
-      </c>
       <c r="D34" t="s">
+        <v>381</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -2790,18 +2790,18 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D36" t="s">
         <v>290</v>
       </c>
       <c r="E36" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>300</v>
       </c>
@@ -2809,21 +2809,21 @@
         <v>299</v>
       </c>
       <c r="E37" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>286</v>
       </c>
       <c r="D38" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E38" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>142</v>
       </c>
@@ -2834,13 +2834,13 @@
         <v>161</v>
       </c>
       <c r="D39" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E39" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>293</v>
       </c>
@@ -2848,21 +2848,21 @@
         <v>294</v>
       </c>
       <c r="E40" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D41" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E41" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>248</v>
       </c>
@@ -2870,10 +2870,10 @@
         <v>285</v>
       </c>
       <c r="E42" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>287</v>
       </c>
@@ -2898,10 +2898,10 @@
         <v>97</v>
       </c>
       <c r="E44" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>292</v>
       </c>
@@ -2909,21 +2909,21 @@
         <v>146</v>
       </c>
       <c r="E45" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" t="s">
         <v>347</v>
       </c>
-      <c r="D46" t="s">
-        <v>348</v>
-      </c>
       <c r="E46" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -2934,24 +2934,24 @@
         <v>281</v>
       </c>
       <c r="D47" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E47" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>284</v>
       </c>
       <c r="D48" t="s">
+        <v>388</v>
+      </c>
+      <c r="E48" t="s">
         <v>389</v>
       </c>
-      <c r="E48" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>282</v>
       </c>
@@ -2959,10 +2959,10 @@
         <v>283</v>
       </c>
       <c r="E49" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>251</v>
       </c>
@@ -2970,12 +2970,12 @@
         <v>250</v>
       </c>
       <c r="E50" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>30</v>
@@ -2987,45 +2987,45 @@
         <v>98</v>
       </c>
       <c r="E51" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
+        <v>315</v>
+      </c>
+      <c r="D52" t="s">
         <v>316</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>317</v>
       </c>
-      <c r="E52" t="s">
+      <c r="D53" t="s">
+        <v>318</v>
+      </c>
+      <c r="E53" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>318</v>
-      </c>
-      <c r="D53" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>319</v>
       </c>
-      <c r="E53" t="s">
+      <c r="D54" t="s">
+        <v>320</v>
+      </c>
+      <c r="E54" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>320</v>
-      </c>
-      <c r="D54" t="s">
-        <v>321</v>
-      </c>
-      <c r="E54" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>29</v>
@@ -3037,21 +3037,21 @@
         <v>99</v>
       </c>
       <c r="E55" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>237</v>
       </c>
       <c r="D56" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>238</v>
       </c>
@@ -3059,10 +3059,10 @@
         <v>239</v>
       </c>
       <c r="E57" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>241</v>
       </c>
@@ -3070,10 +3070,10 @@
         <v>242</v>
       </c>
       <c r="E58" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -3084,48 +3084,48 @@
         <v>151</v>
       </c>
       <c r="D59" t="s">
-        <v>313</v>
+        <v>424</v>
       </c>
       <c r="E59" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
+        <v>321</v>
+      </c>
+      <c r="D60" t="s">
         <v>322</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>323</v>
       </c>
-      <c r="E60" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>324</v>
-      </c>
       <c r="D61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E61" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
+        <v>328</v>
+      </c>
+      <c r="D62" t="s">
         <v>329</v>
-      </c>
-      <c r="D62" t="s">
-        <v>330</v>
       </c>
       <c r="E62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>34</v>
@@ -3137,10 +3137,10 @@
         <v>156</v>
       </c>
       <c r="E63" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>160</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>310</v>
       </c>
@@ -3159,23 +3159,23 @@
         <v>311</v>
       </c>
       <c r="E65" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>312</v>
       </c>
       <c r="D66" t="s">
+        <v>402</v>
+      </c>
+      <c r="E66" t="s">
         <v>403</v>
       </c>
-      <c r="E66" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>35</v>
@@ -3184,13 +3184,13 @@
         <v>236</v>
       </c>
       <c r="D67" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E67" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>154</v>
       </c>
@@ -3198,10 +3198,10 @@
         <v>235</v>
       </c>
       <c r="E68" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>163</v>
       </c>
@@ -3209,10 +3209,10 @@
         <v>162</v>
       </c>
       <c r="E69" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>246</v>
       </c>
@@ -3220,12 +3220,12 @@
         <v>245</v>
       </c>
       <c r="E70" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>33</v>
@@ -3237,10 +3237,10 @@
         <v>96</v>
       </c>
       <c r="E71" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>234</v>
       </c>
@@ -3248,10 +3248,10 @@
         <v>233</v>
       </c>
       <c r="E72" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>244</v>
       </c>
@@ -3259,10 +3259,10 @@
         <v>243</v>
       </c>
       <c r="E73" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>295</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>296</v>
       </c>
       <c r="E74" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -3287,9 +3287,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>166</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>167</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>168</v>
       </c>
@@ -3313,327 +3313,327 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>307</v>
       </c>

</xml_diff>